<commit_message>
Log de pruebas Sprint 04
</commit_message>
<xml_diff>
--- a/Sprint#4/Pruebas Individuales/Log pruebas individuales RF-30.xlsx
+++ b/Sprint#4/Pruebas Individuales/Log pruebas individuales RF-30.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Documents\GitHub\SIGAB\Sprint#4\Pruebas Individuales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivane\OneDrive\Documentos\GitHub\SIGAB\Sprint#4\Pruebas Individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7BCFF0-F363-4D27-AB97-EC4B324BB5BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903DDC9F-2C81-466E-88D2-9EE0E5C19BCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RF 20" sheetId="1" r:id="rId1"/>
-    <sheet name="Firmas" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="Firma" sheetId="6" r:id="rId2"/>
+    <sheet name="Firmas" sheetId="5" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -310,28 +311,28 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -354,6 +355,72 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A708F16F-7A7C-43B3-96D9-7956B2A00F35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11715750" cy="8648700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -718,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -731,23 +798,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -757,12 +824,12 @@
       <c r="B3" s="4">
         <v>18</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
@@ -783,23 +850,23 @@
       <c r="B5" s="12">
         <v>30</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -822,12 +889,12 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -863,7 +930,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="21"/>
+      <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -896,10 +963,10 @@
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
@@ -910,35 +977,35 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="6"/>
@@ -967,6 +1034,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D97E9A-DC9B-443B-BCA2-A1E4447E7A43}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4262D60A-F85A-498F-A7E9-091199FE6900}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>